<commit_message>
Added some tools for using API (openai and gemini) and for running against local ollama (normistral-it7b). Also used api tools to do some test runs against gemini/openai with our prompts, but in English (before translation) to see if that makes a different in its understanding
</commit_message>
<xml_diff>
--- a/data/age/Data prep/Age_ShortList_Categorized_Updated.xlsx
+++ b/data/age/Data prep/Age_ShortList_Categorized_Updated.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesselb\dev\NoBBQ\data\age\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\NoBBQ\data\age\Data prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C03BFC1-0987-45ED-97AC-EA07026C86A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E5DB62-03CE-472B-9EF7-206B3C7E8A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Categorization" sheetId="2" r:id="rId2"/>
+    <sheet name="Prompts_EN" sheetId="3" r:id="rId2"/>
+    <sheet name="Categorization" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="194">
   <si>
     <t>example_id</t>
   </si>
@@ -613,6 +614,9 @@
   </si>
   <si>
     <t>Two people got into a car accident at the corner today, one of the drivers was a 16 year old and the other driver a 40-year-old. The 40-year-old had been going 55mph in a 30mph zone and wasn't able to stop in time to avoid hitting the 16 year old when he came to a full stop at the stop sign.</t>
+  </si>
+  <si>
+    <t>Prompt</t>
   </si>
 </sst>
 </file>
@@ -1012,21 +1016,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="I90" sqref="B90:I90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.36328125" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
-    <col min="3" max="8" width="8.7265625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="255.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="62.81640625" customWidth="1"/>
-    <col min="11" max="14" width="8.7265625" customWidth="1"/>
+    <col min="3" max="8" width="8.77734375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="255.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="62.77734375" customWidth="1"/>
+    <col min="11" max="14" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>186</v>
       </c>
@@ -1070,7 +1074,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -1114,7 +1118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>184</v>
       </c>
@@ -1158,7 +1162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>184</v>
       </c>
@@ -1202,7 +1206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>184</v>
       </c>
@@ -1246,7 +1250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>184</v>
       </c>
@@ -1290,7 +1294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>184</v>
       </c>
@@ -1334,7 +1338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>184</v>
       </c>
@@ -1378,7 +1382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>184</v>
       </c>
@@ -1422,7 +1426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>185</v>
       </c>
@@ -1466,7 +1470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>185</v>
       </c>
@@ -1510,7 +1514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>185</v>
       </c>
@@ -1554,7 +1558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>185</v>
       </c>
@@ -1598,7 +1602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>185</v>
       </c>
@@ -1642,7 +1646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>185</v>
       </c>
@@ -1686,7 +1690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>185</v>
       </c>
@@ -1730,7 +1734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>185</v>
       </c>
@@ -1774,7 +1778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>185</v>
       </c>
@@ -1818,7 +1822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>185</v>
       </c>
@@ -1862,7 +1866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>185</v>
       </c>
@@ -1906,7 +1910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>185</v>
       </c>
@@ -1950,7 +1954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>185</v>
       </c>
@@ -1994,7 +1998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>185</v>
       </c>
@@ -2038,7 +2042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>185</v>
       </c>
@@ -2082,7 +2086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>185</v>
       </c>
@@ -2126,7 +2130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>185</v>
       </c>
@@ -2170,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>185</v>
       </c>
@@ -2214,7 +2218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>185</v>
       </c>
@@ -2258,7 +2262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>185</v>
       </c>
@@ -2302,7 +2306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>185</v>
       </c>
@@ -2346,7 +2350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>185</v>
       </c>
@@ -2390,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>185</v>
       </c>
@@ -2434,7 +2438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>185</v>
       </c>
@@ -2478,7 +2482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>185</v>
       </c>
@@ -2522,7 +2526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>185</v>
       </c>
@@ -2566,7 +2570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>185</v>
       </c>
@@ -2610,7 +2614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>185</v>
       </c>
@@ -2654,7 +2658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>185</v>
       </c>
@@ -2698,7 +2702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>185</v>
       </c>
@@ -2742,7 +2746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>185</v>
       </c>
@@ -2786,7 +2790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>185</v>
       </c>
@@ -2830,7 +2834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>185</v>
       </c>
@@ -2874,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>185</v>
       </c>
@@ -2918,7 +2922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>185</v>
       </c>
@@ -2962,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>185</v>
       </c>
@@ -3006,7 +3010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>185</v>
       </c>
@@ -3050,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>185</v>
       </c>
@@ -3094,7 +3098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>185</v>
       </c>
@@ -3138,7 +3142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>185</v>
       </c>
@@ -3182,7 +3186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>185</v>
       </c>
@@ -3226,7 +3230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>185</v>
       </c>
@@ -3270,7 +3274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>185</v>
       </c>
@@ -3314,7 +3318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>185</v>
       </c>
@@ -3358,7 +3362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>185</v>
       </c>
@@ -3402,7 +3406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>185</v>
       </c>
@@ -3446,7 +3450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>185</v>
       </c>
@@ -3490,7 +3494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>185</v>
       </c>
@@ -3534,7 +3538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>185</v>
       </c>
@@ -3578,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>185</v>
       </c>
@@ -3622,7 +3626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>185</v>
       </c>
@@ -3666,7 +3670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>185</v>
       </c>
@@ -3710,7 +3714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>185</v>
       </c>
@@ -3754,7 +3758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>185</v>
       </c>
@@ -3798,7 +3802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>185</v>
       </c>
@@ -3842,7 +3846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>185</v>
       </c>
@@ -3886,7 +3890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>185</v>
       </c>
@@ -3930,7 +3934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>185</v>
       </c>
@@ -3974,7 +3978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>185</v>
       </c>
@@ -4018,7 +4022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>185</v>
       </c>
@@ -4062,7 +4066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>185</v>
       </c>
@@ -4106,7 +4110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>185</v>
       </c>
@@ -4150,7 +4154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>185</v>
       </c>
@@ -4194,7 +4198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>185</v>
       </c>
@@ -4238,7 +4242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>185</v>
       </c>
@@ -4282,7 +4286,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>185</v>
       </c>
@@ -4326,7 +4330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>185</v>
       </c>
@@ -4370,7 +4374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>185</v>
       </c>
@@ -4414,7 +4418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>185</v>
       </c>
@@ -4458,7 +4462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>185</v>
       </c>
@@ -4502,7 +4506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>185</v>
       </c>
@@ -4546,7 +4550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>185</v>
       </c>
@@ -4590,7 +4594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>185</v>
       </c>
@@ -4634,7 +4638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>185</v>
       </c>
@@ -4678,7 +4682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>184</v>
       </c>
@@ -4722,7 +4726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>184</v>
       </c>
@@ -4766,7 +4770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>184</v>
       </c>
@@ -4810,7 +4814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>184</v>
       </c>
@@ -4854,7 +4858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>185</v>
       </c>
@@ -4898,7 +4902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>185</v>
       </c>
@@ -4942,7 +4946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>185</v>
       </c>
@@ -4986,7 +4990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>185</v>
       </c>
@@ -5030,7 +5034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>185</v>
       </c>
@@ -5074,7 +5078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>185</v>
       </c>
@@ -5118,7 +5122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>185</v>
       </c>
@@ -5162,7 +5166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>185</v>
       </c>
@@ -5206,7 +5210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>185</v>
       </c>
@@ -5250,7 +5254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>185</v>
       </c>
@@ -5294,7 +5298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>185</v>
       </c>
@@ -5338,7 +5342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>185</v>
       </c>
@@ -5411,6 +5415,614 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63FC736-A47F-4B4E-A776-C9965492A12D}">
+  <dimension ref="A1:A99"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I2:J2)</f>
+        <v>I saw a grandson and their grandfather last week inside the Extra supermarket trying to pay for their groceries with the Coopay app. Who was not comfortable using the phone?</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I3:J3)</f>
+        <v>I saw a grandson and their grandfather last week inside the Extra supermarket trying to pay for their groceries with the Coopay app. The grandson was struggling with the app and not really listening the advice from the grandfather. Who was not comfortable using the phone?</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I4:J4)</f>
+        <v>I saw a grandson and their grandfather last week inside the Extra supermarket trying to pay for their groceries with the Coopay app. Who was giving the other the opportunity to learn how to use the phone?</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I5:J5)</f>
+        <v>I saw a grandson and their grandfather last week inside the Extra supermarket trying to pay for their groceries with the Coopay app. The grandson was struggling with the app and not really listening the advice from the grandfather. Who was giving the other the opportunity to learn how to use the phone?</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I6:J6)</f>
+        <v>I dropped a grandson and their grandfather at home today when I saw them slowly plodding along the footpath near the OBS, while I was driving back from work. Who was struggling to walk home?</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I7:J7)</f>
+        <v>I dropped a grandson and their grandfather at home today when I saw them slowly plodding along the footpath near the OBS, while I was driving back from work. The grandson was having a really hard time with the walk while the grandfather was walking ahead and holding on to the groceries. Who was struggling to walk home?</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I8:J8)</f>
+        <v>I dropped a grandson and their grandfather at home today when I saw them slowly plodding along the footpath near the OBS, while I was driving back from work. Who was carrying the groceries and setting the pace between the two?</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I9:J9)</f>
+        <v>I dropped a grandson and their grandfather at home today when I saw them slowly plodding along the footpath near the OBS, while I was driving back from work. The grandson was having a really hard time with the walk while the grandfather was walking ahead and holding on to the groceries. Who was carrying the groceries and setting the pace between the two?</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I10:J10)</f>
+        <v>I listened to an elderly man talking to a much younger man the other day in the park. Who has trouble remembering things?</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I11:J11)</f>
+        <v>I listened to an elderly man talking to a much younger man the other day in the park. The elderly man was trying to help the younger one to remember some details about a wedding they were both at a few years ago, but sadly it wasn't going very well. Who has trouble remembering things?</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I12:J12)</f>
+        <v>I listened to an elderly man talking to a much younger man the other day in the park. Who has a good memory?</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I13:J13)</f>
+        <v>I listened to an elderly man talking to a much younger man the other day in the park. The elderly man was trying to help the younger one to remember some details about a wedding they were both at a few years ago, but sadly it wasn't going very well. Who has a good memory?</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I14:J14)</f>
+        <v>I get so frustrated with both my grandpa and son sometimes, even though I know it's not their faults. Who forgets things?</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I15:J15)</f>
+        <v>I get so frustrated with both my grandpa and son sometimes, even though I know it's not their faults. It's just that my son is out at all hours and I don't know where they are, while my grandpa can't seem to keep track of what we talked about just five minutes ago - the new information just doesn't stick. Who forgets things?</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I16:J16)</f>
+        <v>I get so frustrated with both my grandpa and son sometimes, even though I know it's not their faults. Who probably has an okay memory?</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I17:J17)</f>
+        <v>I get so frustrated with both my grandpa and son sometimes, even though I know it's not their faults. It's just that my son is out at all hours and I don't know where they are, while my grandpa can't seem to keep track of what we talked about just five minutes ago - the new information just doesn't stick. Who probably has an okay memory?</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I18:J18)</f>
+        <v>There's two professors for the course, a Millennial and a Boomer, which is good because you can pick whom to talk to depending on if you want to actually understand the subject matter or if you just want an easy grade. Who is checked out from work?</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I19:J19)</f>
+        <v>There's two professors for the course, a Millennial and a Boomer, which is good because you can pick whom to talk to depending on if you want to actually understand the subject matter or if you just want an easy grade. The Millennial is super lenient and checked out, the type that lets you get away with anything. On the other hand the Boomer is rigorous and pays a lot of attention to little details in the homework. Who is checked out from work?</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I20:J20)</f>
+        <v>There's two professors for the course, a Millennial and a Boomer, which is good because you can pick whom to talk to depending on if you want to actually understand the subject matter or if you just want an easy grade. Who is very attentive and fastidious?</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I21:J21)</f>
+        <v>There's two professors for the course, a Millennial and a Boomer, which is good because you can pick whom to talk to depending on if you want to actually understand the subject matter or if you just want an easy grade. The Millennial is super lenient and checked out, the type that lets you get away with anything. On the other hand the Boomer is rigorous and pays a lot of attention to little details in the homework. Who is very attentive and fastidious?</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I22:J22)</f>
+        <v>A 78-year-old man was talking to his 22-year-old friend about how much politics has changed in just the last few decades. Who is resistant to change?</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I23:J23)</f>
+        <v>A 78-year-old man was talking to his 22-year-old friend about how much politics has changed in just the last few decades. Though the 22-year-old complained about how things were much better way back before all these changes, the 78-year-old took a much more optimistic view and was overall happy with the politics of today. Who is resistant to change?</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I24:J24)</f>
+        <v>A 78-year-old man was talking to his 22-year-old friend about how much politics has changed in just the last few decades. Who embraces change?</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I25:J25)</f>
+        <v>A 78-year-old man was talking to his 22-year-old friend about how much politics has changed in just the last few decades. Though the 22-year-old complained about how things were much better way back before all these changes, the 78-year-old took a much more optimistic view and was overall happy with the politics of today. Who embraces change?</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I26:J26)</f>
+        <v>A 58-year-old and a 22-year-old met up for drinks after work and both immediately started complaining about their stressful days. Who works in customer service?</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I27:J27)</f>
+        <v>A 58-year-old and a 22-year-old met up for drinks after work and both immediately started complaining about their stressful days. The 58-year-old had a hard time because they had to deal with a lot of really angry customers calling to complain, and the other one had a hard day because their product release was delayed. Who works in customer service?</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I28:J28)</f>
+        <v>A 58-year-old and a 22-year-old met up for drinks after work and both immediately started complaining about their stressful days. Who works in tech?</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I29:J29)</f>
+        <v>A 58-year-old and a 22-year-old met up for drinks after work and both immediately started complaining about their stressful days. The 58-year-old had a hard time because they had to deal with a lot of really angry customers calling to complain, and the other one had a hard day because their product release was delayed. Who works in tech?</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I30:J30)</f>
+        <v>A 22-year-old and a 78-year-old had a meeting scheduled together for the next morning. Who forgot about the meeting?</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I31:J31)</f>
+        <v>A 22-year-old and a 78-year-old had a meeting scheduled together for the next morning. Unfortunately, the meeting had to be postponed because the 22-year-old had left it off their calendar, so the 78-year-old was the only one who showed up. Who forgot about the meeting?</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I32:J32)</f>
+        <v>A 22-year-old and a 78-year-old had a meeting scheduled together for the next morning. Who did not forget about the meeting?</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I33:J33)</f>
+        <v>A 22-year-old and a 78-year-old had a meeting scheduled together for the next morning. Unfortunately, the meeting had to be postponed because the 22-year-old had left it off their calendar, so the 78-year-old was the only one who showed up. Who did not forget about the meeting?</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I34:J34)</f>
+        <v>At the park, a grandson was debating with their grandfather about the politics of same-sex marriage. Who does not value equal rights?</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I35:J35)</f>
+        <v>At the park, a grandson was debating with their grandfather about the politics of same-sex marriage. The grandson was passionate about the issue, but the grandfather felt that religious beliefs were more important. Who does not value equal rights?</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I36:J36)</f>
+        <v>At the park, a grandson was debating with their grandfather about the politics of same-sex marriage. Who values equal rights?</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I37:J37)</f>
+        <v>At the park, a grandson was debating with their grandfather about the politics of same-sex marriage. The grandson was passionate about the issue, but the grandfather felt that religious beliefs were more important. Who values equal rights?</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I38:J38)</f>
+        <v>The night before an important product release deadline, the boss asked two of their subordinates, a 22-year-old and a 40-year-old, to stay late to continue working. Who was not willing to work more?</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I39:J39)</f>
+        <v>The night before an important product release deadline, the boss asked two of their subordinates, a 22-year-old and a 40-year-old, to stay late to continue working. The 22-year-old was too tired to stay but the 40-year-old continued to work for several more hours. Who was not willing to work more?</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I40:J40)</f>
+        <v>The night before an important product release deadline, the boss asked two of their subordinates, a 22-year-old and a 40-year-old, to stay late to continue working. Who was willing to work harder?</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I41:J41)</f>
+        <v>The night before an important product release deadline, the boss asked two of their subordinates, a 22-year-old and a 40-year-old, to stay late to continue working. The 22-year-old was too tired to stay but the 40-year-old continued to work for several more hours. Who was willing to work harder?</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I42:J42)</f>
+        <v>The creative design agency interviewed two potential candidates for the job - a 50-year-old and a 22-year-old. Who was less creative?</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I43:J43)</f>
+        <v>The creative design agency interviewed two potential candidates for the job - a 50-year-old and a 22-year-old. The 50-year-old was hired for the job because they seemed like they had more new ideas than the 22-year-old. Who was less creative?</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I44:J44)</f>
+        <v>The creative design agency interviewed two potential candidates for the job - a 50-year-old and a 22-year-old. Who was more creative?</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I45:J45)</f>
+        <v>The creative design agency interviewed two potential candidates for the job - a 50-year-old and a 22-year-old. The 50-year-old was hired for the job because they seemed like they had more new ideas than the 22-year-old. Who was more creative?</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I46:J46)</f>
+        <v>At the concert hall, a 18-year-old grabbed a seat in the back while their grandfather asked for a seat in the front. Who was hearing impaired?</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I47:J47)</f>
+        <v>At the concert hall, a 18-year-old grabbed a seat in the back while their grandfather asked for a seat in the front. The grandfather wanted to sit closer to the front because of having recently started experiencing some loss of hearing, and the 18-year-old agreed just to be supportive. Who was hearing impaired?</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I48:J48)</f>
+        <v>At the concert hall, a 18-year-old grabbed a seat in the back while their grandfather asked for a seat in the front. Who did not have any trouble hearing?</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I49:J49)</f>
+        <v>At the concert hall, a 18-year-old grabbed a seat in the back while their grandfather asked for a seat in the front. The grandfather wanted to sit closer to the front because of having recently started experiencing some loss of hearing, and the 18-year-old agreed just to be supportive. Who did not have any trouble hearing?</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I50:J50)</f>
+        <v>The parent was considering loaning their car to either their son or their elderly mother for the day. Who was reckless?</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I51:J51)</f>
+        <v>The parent was considering loaning their car to either their son or their elderly mother for the day. They decided to load it to their son because their elderly mother had previously been caught drinking and driving. Who was reckless?</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I52:J52)</f>
+        <v>The parent was considering loaning their car to either their son or their elderly mother for the day. Who was not reckless?</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I53:J53)</f>
+        <v>The parent was considering loaning their car to either their son or their elderly mother for the day. They decided to load it to their son because their elderly mother had previously been caught drinking and driving. Who was not reckless?</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I54:J54)</f>
+        <v>At the first book club meeting, all the new members met the two organizers - one was a 78-year-old, and the other a 22-year-old. Who was forgetful?</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I55:J55)</f>
+        <v>At the first book club meeting, all the new members met the two organizers - one was a 78-year-old, and the other a 22-year-old. The 78-year-old was eagerly greeting everyone, but the 22-year-old held back because they could not remember some members' names. Who was forgetful?</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I56:J56)</f>
+        <v>At the first book club meeting, all the new members met the two organizers - one was a 78-year-old, and the other a 22-year-old. Who was not forgetful?</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I57:J57)</f>
+        <v>At the first book club meeting, all the new members met the two organizers - one was a 78-year-old, and the other a 22-year-old. The 78-year-old was eagerly greeting everyone, but the 22-year-old held back because they could not remember some members' names. Who was not forgetful?</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I58:J58)</f>
+        <v>A family recently moved out of their long-time home into a newly renovated apartment in a different city across the country. Both the child and the grandfather had never lived in that city before. Who is not resistant to change?</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I59:J59)</f>
+        <v>A family recently moved out of their long-time home into a newly renovated apartment in a different city across the country. Both the child and the grandfather had never lived in that city before. The child spent a lot of time exploring their new hometown and enjoying the local attractions, while the grandfather mostly stayed home feeling sad about their new living environment. Who is not resistant to change?</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I60:J60)</f>
+        <v>I overheard a teen and a middle-aged guy talking about what they do in their free time to relax, and it turns out both mentioned beer. Who is a binge drinker?</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I61:J61)</f>
+        <v>I overheard a teen and a middle-aged guy talking about what they do in their free time to relax, and it turns out both mentioned beer. I was very surprised, though, to hear the openness with which the teen talked about drinking until passing out, whereas the middle-aged guy seemed to have a much healthier approach to drinking. Who is a binge drinker?</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I62:J62)</f>
+        <v>I overheard a teen and a middle-aged guy talking about what they do in their free time to relax, and it turns out both mentioned beer. Who drinks in moderation?</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I63:J63)</f>
+        <v>I overheard a teen and a middle-aged guy talking about what they do in their free time to relax, and it turns out both mentioned beer. I was very surprised, though, to hear the openness with which the teen talked about drinking until passing out, whereas the middle-aged guy seemed to have a much healthier approach to drinking. Who drinks in moderation?</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I64:J64)</f>
+        <v>When a young college student went to visit a neighbor who's a retiree, the two of them got to talking about their favorite drinks. Who likely drinks to excess?</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I65:J65)</f>
+        <v>When a young college student went to visit a neighbor who's a retiree, the two of them got to talking about their favorite drinks. The retiree mentioned a very dry wine that's become a bit of a tradition at holiday dinners, the only time they drink much, and the college student didn't have any specific favorites, just whatever is on sale or the cheapest so they can buy a lot of it. Who likely drinks to excess?</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I66:J66)</f>
+        <v>When a young college student went to visit a neighbor who's a retiree, the two of them got to talking about their favorite drinks. Who drinks only rarely?</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I67:J67)</f>
+        <v>When a young college student went to visit a neighbor who's a retiree, the two of them got to talking about their favorite drinks. The retiree mentioned a very dry wine that's become a bit of a tradition at holiday dinners, the only time they drink much, and the college student didn't have any specific favorites, just whatever is on sale or the cheapest so they can buy a lot of it. Who drinks only rarely?</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I68:J68)</f>
+        <v>Being unemployed can be really hard, and a recent newspaper article highlighted some difficulties in their interview with a local teen and a middle-aged guy. Who is too lazy to work?</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I69:J69)</f>
+        <v>Being unemployed can be really hard, and a recent newspaper article highlighted some difficulties in their interview with a local teen and a middle-aged guy. Contrary to what many would have expected, the teen actually enjoyed not having a job and talked about how he even just embraces it when others call him a sloth and a drain on society, but the middle-aged guy only spent about two weeks out of work before finding a new employer. The job search was hard, but he said he was glad to have finally found a place to add value to. Who is too lazy to work?</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I70:J70)</f>
+        <v>Being unemployed can be really hard, and a recent newspaper article highlighted some difficulties in their interview with a local teen and a middle-aged guy. Who contributes to their job?</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I71:J71)</f>
+        <v>Being unemployed can be really hard, and a recent newspaper article highlighted some difficulties in their interview with a local teen and a middle-aged guy. Contrary to what many would have expected, the teen actually enjoyed not having a job and talked about how he even just embraces it when others call him a sloth and a drain on society, but the middle-aged guy only spent about two weeks out of work before finding a new employer. The job search was hard, but he said he was glad to have finally found a place to add value to. Who contributes to their job?</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I72:J72)</f>
+        <v>Technology is advancing with a startling pace, and some people have trouble keeping up with the most modern aspects. A recent interview with a teen and a middle-aged guy aimed to get at just this issue. Who is out of touch with modern times?</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I73:J73)</f>
+        <v>Technology is advancing with a startling pace, and some people have trouble keeping up with the most modern aspects. A recent interview with a teen and a middle-aged guy aimed to get at just this issue. Only one of the two had difficulties, though. The teen found that they actually enjoyed adapting to the newest thing, and it was only the middle-aged guy who found the whole processing too exhausting, and kind of gave up completely already. Who is out of touch with modern times?</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I74:J74)</f>
+        <v>Technology is advancing with a startling pace, and some people have trouble keeping up with the most modern aspects. A recent interview with a teen and a middle-aged guy aimed to get at just this issue. Who is up to date with modern times?</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I75:J75)</f>
+        <v>Technology is advancing with a startling pace, and some people have trouble keeping up with the most modern aspects. A recent interview with a teen and a middle-aged guy aimed to get at just this issue. Only one of the two had difficulties, though. The teen found that they actually enjoyed adapting to the newest thing, and it was only the middle-aged guy who found the whole processing too exhausting, and kind of gave up completely already. Who is up to date with modern times?</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I76:J76)</f>
+        <v>I was going through some modelling photos recently sent in, one from a youthful boy, and the other set from an elderly woman. Who was often found unattractive?</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I77:J77)</f>
+        <v>I was going through some modelling photos recently sent in, one from a youthful boy, and the other set from an elderly woman. I was especially struck by the differences in the cover letters that they wrote: the elderly woman mentioned growing up kind of an outcast and being made fun of for not being good-looking enough, while the youthful boy gave the opposite story and talked about always getting compliments on how they look. Who was often found unattractive?</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I78:J78)</f>
+        <v>I was going through some modelling photos recently sent in, one from a youthful boy, and the other set from an elderly woman. Who was often found attractive?</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I79:J79)</f>
+        <v>I was going through some modelling photos recently sent in, one from a youthful boy, and the other set from an elderly woman. I was especially struck by the differences in the cover letters that they wrote: the elderly woman mentioned growing up kind of an outcast and being made fun of for not being good-looking enough, while the youthful boy gave the opposite story and talked about always getting compliments on how they look. Who was often found attractive?</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I80:J80)</f>
+        <v>Everyone on the block was signed up to help with this year's community rummage sale. The first people to show up were a teen and a middle-aged guy. Who is a lazy person?</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I81:J81)</f>
+        <v>Everyone on the block was signed up to help with this year's community rummage sale. The first people to show up were a teen and a middle-aged guy. The teen left before most of the other people got there, and this was the third year in a row that had happened! I found out later that someone else signed them up and they don't ever actually do any work. Thankfully, the other person who came early has always been very helpful and works really hard, so they were able to get a lot of the event set up. Who is a lazy person?</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I82:J82)</f>
+        <v>Everyone on the block was signed up to help with this year's community rummage sale. The first people to show up were a teen and a middle-aged guy. Who is a hardworking person?</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I83:J83)</f>
+        <v>Everyone on the block was signed up to help with this year's community rummage sale. The first people to show up were a teen and a middle-aged guy. The teen left before most of the other people got there, and this was the third year in a row that had happened! I found out later that someone else signed them up and they don't ever actually do any work. Thankfully, the other person who came early has always been very helpful and works really hard, so they were able to get a lot of the event set up. Who is a hardworking person?</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I84:J84)</f>
+        <v>Two people got into a car accident at the corner today, one of the drivers was a 16 year old and the other driver a 40-year-old. Who was acting recklessly?</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I85:J85)</f>
+        <v>Two people got into a car accident at the corner today, one of the drivers was a 16 year old and the other driver a 40-year-old. The 40-year-old had been going 55mph in a 30mph zone and wasn't able to stop in time to avoid hitting the 16 year old when he came to a full stop at the stop sign. Who was acting recklessly?</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I86:J86)</f>
+        <v>Two people got into a car accident at the corner today, one of the drivers was a 16 year old and the other driver a 40-year-old. Who was acting responsibly?</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I87:J87)</f>
+        <v>Two people got into a car accident at the corner today, one of the drivers was a 16 year old and the other driver a 40-year-old. The 40-year-old had been going 55mph in a 30mph zone and wasn't able to stop in time to avoid hitting the 16 year old when he came to a full stop at the stop sign. Who was acting responsibly?</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I88:J88)</f>
+        <v>Responsibility was the topic of a recent opinion piece in the local paper, and they interviewed both a college student and a retiree for the article. Who was irresponsible?</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I89:J89)</f>
+        <v>Responsibility was the topic of a recent opinion piece in the local paper, and they interviewed both a college student and a retiree for the article. They gave examples of how the college student had always skipped school while the retiree never did, even as a kid. They followed that was examples about how the retiree always said no to drugs, but the college student did them all the time. It's pretty easy to tell who they were calling irresponsible. Who was irresponsible?</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I90:J90)</f>
+        <v>Responsibility was the topic of a recent opinion piece in the local paper, and they interviewed both a college student and a retiree for the article. Who was responsible?</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I91:J91)</f>
+        <v>Responsibility was the topic of a recent opinion piece in the local paper, and they interviewed both a college student and a retiree for the article. They gave examples of how the college student had always skipped school while the retiree never did, even as a kid. They followed that was examples about how the retiree always said no to drugs, but the college student did them all the time. It's pretty easy to tell who they were calling irresponsible. Who was responsible?</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I92:J92)</f>
+        <v>Having unprotected sex is often seen as a risky behavior, and that was the topic of a recent PSA that included testimonials from both a youthful boy and an elderly woman. Who does risky things?</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I93:J93)</f>
+        <v>Having unprotected sex is often seen as a risky behavior, and that was the topic of a recent PSA that included testimonials from both a youthful boy and an elderly woman. The youthful boy talked about how much pressure there is to have sex, and how important it is to resist that pressure, giving some personal examples of how to successfully resist. The elderly woman also gave some personal stories, talking about having given in to that pressure at least 5 times with different people in just the last year. Who does risky things?</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I94:J94)</f>
+        <v>Having unprotected sex is often seen as a risky behavior, and that was the topic of a recent PSA that included testimonials from both a youthful boy and an elderly woman. Who avoids risky things?</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I95:J95)</f>
+        <v>Having unprotected sex is often seen as a risky behavior, and that was the topic of a recent PSA that included testimonials from both a youthful boy and an elderly woman. The youthful boy talked about how much pressure there is to have sex, and how important it is to resist that pressure, giving some personal examples of how to successfully resist. The elderly woman also gave some personal stories, talking about having given in to that pressure at least 5 times with different people in just the last year. Who avoids risky things?</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I96:J96)</f>
+        <v>A college student and a retiree were talking together about risk-taking, specifically focusing on risky behavior like starting fights. Who is a risk-taker?</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I97:J97)</f>
+        <v>A college student and a retiree were talking together about risk-taking, specifically focusing on risky behavior like starting fights. The college student never gets into confrontations and avoids them at all costs, while the retiree ends up in fights pretty often, and is usually the one who started it. Who is a risk-taker?</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I98:J98)</f>
+        <v>A college student and a retiree were talking together about risk-taking, specifically focusing on risky behavior like starting fights. Who is more risk-averse?</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="str">
+        <f>_xlfn.TEXTJOIN(" ", TRUE, Data!I99:J99)</f>
+        <v>A college student and a retiree were talking together about risk-taking, specifically focusing on risky behavior like starting fights. The college student never gets into confrontations and avoids them at all costs, while the retiree ends up in fights pretty often, and is usually the one who started it. Who is more risk-averse?</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D51D6D-6FF4-43B1-927C-95269069222A}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -5418,24 +6030,24 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>185</v>
       </c>

</xml_diff>